<commit_message>
updates features and consistency
</commit_message>
<xml_diff>
--- a/e.g/bd.xlsx
+++ b/e.g/bd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.lourenco\Documents\GitHub\GSDA-310\e.g\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A19800-9DED-48F3-B08A-BD5F25045A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5819755-4C16-4E78-92B8-9BF6830DD050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="2160" windowWidth="22980" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3570" yWindow="2145" windowWidth="22980" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,8 +407,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <f ca="1">TODAY()</f>
-        <v>45579</v>
+        <v>37593</v>
       </c>
       <c r="C2" s="2">
         <v>0.36319444444444443</v>
@@ -422,7 +421,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>45270</v>
+        <v>38343</v>
       </c>
       <c r="C3" s="2">
         <v>0.8125</v>

</xml_diff>

<commit_message>
updates class <To> and its methods
</commit_message>
<xml_diff>
--- a/e.g/bd.xlsx
+++ b/e.g/bd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.lourenco\Documents\GitHub\GSDA-310\e.g\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5819755-4C16-4E78-92B8-9BF6830DD050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F3A862-5669-483B-A70D-AEC6DB6C8E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="2145" windowWidth="22980" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="2505" windowWidth="22980" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E3" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Encountered a necessity to update the zip feature - further updates gonna be necessary
</commit_message>
<xml_diff>
--- a/e.g/bd.xlsx
+++ b/e.g/bd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.lourenco\Documents\GitHub\GSDA-310\e.g\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F3A862-5669-483B-A70D-AEC6DB6C8E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBC4525-0958-4106-A183-FFA3182E2C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2505" windowWidth="22980" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>NAME</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Maria Mencari</t>
+  </si>
+  <si>
+    <t>VALUE</t>
   </si>
 </sst>
 </file>
@@ -376,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E1:E1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +391,7 @@
     <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,8 +404,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -415,8 +421,11 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2">
+        <v>99999</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -428,6 +437,9 @@
       </c>
       <c r="D3" t="s">
         <v>5</v>
+      </c>
+      <c r="E3">
+        <v>55555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>